<commit_message>
Added data to sample model file
</commit_message>
<xml_diff>
--- a/sample_model.xlsx
+++ b/sample_model.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nirvana/Documents/Github/Excel-parser-for-cobrapy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61D49CB0-17E4-924C-9B15-D4972F5A280F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE4B047-5A20-4E45-AC88-B38438D2601F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="1320" windowWidth="27060" windowHeight="16940" xr2:uid="{A1B3372C-D0E2-0049-AFEC-AFD004B7E0E2}"/>
+    <workbookView xWindow="5640" yWindow="2120" windowWidth="27060" windowHeight="16940" activeTab="1" xr2:uid="{A1B3372C-D0E2-0049-AFEC-AFD004B7E0E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Reaction List" sheetId="1" r:id="rId1"/>
+    <sheet name="Metabolite List" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,6 +33,119 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Reaction</t>
+  </si>
+  <si>
+    <t>GPR</t>
+  </si>
+  <si>
+    <t>Genes</t>
+  </si>
+  <si>
+    <t>Proteins</t>
+  </si>
+  <si>
+    <t>Subsystem</t>
+  </si>
+  <si>
+    <t>Reversible</t>
+  </si>
+  <si>
+    <t>Lower bound</t>
+  </si>
+  <si>
+    <t>Upper bound</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Confidence</t>
+  </si>
+  <si>
+    <t>EC Number</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Neutral formula</t>
+  </si>
+  <si>
+    <t>Charged formula</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Compartment</t>
+  </si>
+  <si>
+    <t>KEGG ID</t>
+  </si>
+  <si>
+    <t>PubChem ID</t>
+  </si>
+  <si>
+    <t>ChEBI ID</t>
+  </si>
+  <si>
+    <t>InChI string</t>
+  </si>
+  <si>
+    <t>SMILES</t>
+  </si>
+  <si>
+    <t>HMDB ID</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; B</t>
+  </si>
+  <si>
+    <t>A + B -&gt; C</t>
+  </si>
+  <si>
+    <t>C -&gt;</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -65,8 +179,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,12 +496,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1E24E1-7B96-C54F-B30E-32AEF7E64A15}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>-10</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFE9698-E408-8147-AE74-61B55CC01E4A}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>